<commit_message>
Update dataprovider method to Util class
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -41,6 +42,18 @@
   </si>
   <si>
     <t xml:space="preserve">Customer added successfully</t>
+  </si>
+  <si>
+    <t xml:space="preserve">customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">currency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Huyen Ha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VND</t>
   </si>
 </sst>
 </file>
@@ -161,7 +174,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -209,4 +222,47 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Setup runmode for testsuite
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="test_suite" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -84,6 +85,27 @@
   </si>
   <si>
     <t xml:space="preserve">Rupee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TestCase_ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runmode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AddCustomerTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OpenAccountTest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
   </si>
 </sst>
 </file>
@@ -93,7 +115,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -126,6 +148,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11.5"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans Mono"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -172,7 +201,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -182,6 +211,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,7 +237,7 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -304,7 +337,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -354,4 +387,64 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update DataProvider with HashTable
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="AddCustomerTest" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="29">
   <si>
     <t xml:space="preserve">firstname</t>
   </si>
@@ -36,6 +36,9 @@
     <t xml:space="preserve">alerttext</t>
   </si>
   <si>
+    <t xml:space="preserve">runmode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huyen</t>
   </si>
   <si>
@@ -45,6 +48,9 @@
     <t xml:space="preserve">Customer added successfully</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Raman</t>
   </si>
   <si>
@@ -60,6 +66,9 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">c</t>
   </si>
   <si>
@@ -96,16 +105,10 @@
     <t xml:space="preserve">BankManagerLoginTest</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">AddCustomerTest</t>
   </si>
   <si>
     <t xml:space="preserve">OpenAccountTest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
   </si>
 </sst>
 </file>
@@ -235,10 +238,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -261,61 +264,76 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>98033</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
+      <c r="E3" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>9</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -334,48 +352,59 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -396,7 +425,7 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -408,34 +437,34 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>